<commit_message>
Web + WPF + IAM + Postman
</commit_message>
<xml_diff>
--- a/CQRS - Use Case.xlsx
+++ b/CQRS - Use Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Backup\POS\Projetos\ProjetoPetShop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6B0763C-4A15-422E-8B19-3A0DA4B99BAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889EA657-25F9-4A84-B5D1-06DF516EBEED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="615" windowWidth="19440" windowHeight="15150" xr2:uid="{F6CE3401-03D6-4B3F-AB31-AB06011BD6F8}"/>
   </bookViews>
@@ -198,15 +198,6 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -218,6 +209,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -548,45 +548,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>